<commit_message>
Extent 5 Chnages and Merged code
</commit_message>
<xml_diff>
--- a/Data Files/TestData.xlsx
+++ b/Data Files/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhak\Accessweb_newextent\AccessWeb\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC5EB38-1462-4551-BDF5-1613750DC9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B50F93B-85DA-4EEB-948D-33A0FACF3A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="954" firstSheet="29" activeTab="32" xr2:uid="{C6F85985-84AE-4DCB-8550-9B2F16782E4E}"/>
+    <workbookView xWindow="2124" yWindow="2124" windowWidth="17280" windowHeight="9036" tabRatio="954" firstSheet="29" activeTab="31" xr2:uid="{C6F85985-84AE-4DCB-8550-9B2F16782E4E}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessWeb" sheetId="53" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3576" uniqueCount="1176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3611" uniqueCount="1183">
   <si>
     <t>username</t>
   </si>
@@ -3618,6 +3618,27 @@
   </si>
   <si>
     <t xml:space="preserve">List View-Folder upload in Files Section - Verify that user is able to choose a folder while uploading </t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>Test to create profile for DynamicInComplete - Duplicate</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Test to create profile for Optistruct - Duplicate</t>
+  </si>
+  <si>
+    <t>Test to create profile for RADIOSS-SMP - Duplicate</t>
+  </si>
+  <si>
+    <t>Test to create profile for RegularInComplete - Duplicate</t>
+  </si>
+  <si>
+    <t>Test to create profile for ShellScript - Duplicate</t>
   </si>
 </sst>
 </file>
@@ -3783,7 +3804,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3820,6 +3841,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -9257,10 +9282,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9872,6 +9897,121 @@
       </c>
       <c r="G26" s="13" t="s">
         <v>615</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>885</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>890</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>877</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>882</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="22" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>1178</v>
       </c>
     </row>
   </sheetData>
@@ -11535,8 +11675,8 @@
   </sheetPr>
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="B53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11874,7 +12014,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>220</v>
       </c>
@@ -12495,7 +12635,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>169</v>
       </c>
@@ -12587,7 +12727,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="1.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>173</v>
       </c>
@@ -12633,7 +12773,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>175</v>
       </c>
@@ -12748,7 +12888,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>345</v>
       </c>
@@ -12771,7 +12911,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>592</v>
       </c>
@@ -12791,18 +12931,18 @@
         <v>2</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>593</v>
       </c>
       <c r="B55" s="17" t="s">
         <v>590</v>
       </c>
-      <c r="C55" s="15" t="s">
-        <v>90</v>
+      <c r="C55" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>11</v>
@@ -12813,19 +12953,19 @@
       <c r="F55" s="16" t="s">
         <v>591</v>
       </c>
-      <c r="G55" s="15" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G55" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>593</v>
       </c>
       <c r="B56" s="17" t="s">
         <v>590</v>
       </c>
-      <c r="C56" s="15" t="s">
-        <v>90</v>
+      <c r="C56" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>11</v>
@@ -12836,11 +12976,11 @@
       <c r="F56" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="G56" s="15" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G56" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>915</v>
       </c>
@@ -12863,7 +13003,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>916</v>
       </c>
@@ -12886,7 +13026,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>917</v>
       </c>
@@ -12909,7 +13049,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>918</v>
       </c>
@@ -12932,7 +13072,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>918</v>
       </c>
@@ -12955,7 +13095,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>919</v>
       </c>
@@ -12978,7 +13118,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>920</v>
       </c>
@@ -13001,7 +13141,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>921</v>
       </c>
@@ -13024,7 +13164,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>922</v>
       </c>
@@ -13047,7 +13187,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>923</v>
       </c>
@@ -13070,7 +13210,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>918</v>
       </c>
@@ -13093,7 +13233,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>924</v>
       </c>
@@ -13116,7 +13256,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>925</v>
       </c>
@@ -13139,7 +13279,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>926</v>
       </c>
@@ -13162,7 +13302,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>927</v>
       </c>
@@ -13185,7 +13325,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>928</v>
       </c>
@@ -13208,7 +13348,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>929</v>
       </c>
@@ -13231,7 +13371,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>930</v>
       </c>
@@ -13254,7 +13394,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>931</v>
       </c>
@@ -13277,7 +13417,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>932</v>
       </c>
@@ -13300,7 +13440,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>933</v>
       </c>
@@ -13323,7 +13463,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>933</v>
       </c>
@@ -13346,7 +13486,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>934</v>
       </c>
@@ -13369,7 +13509,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>935</v>
       </c>
@@ -13392,7 +13532,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>936</v>
       </c>
@@ -13415,7 +13555,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
         <v>937</v>
       </c>
@@ -13438,7 +13578,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>938</v>
       </c>
@@ -13461,7 +13601,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>939</v>
       </c>
@@ -13484,7 +13624,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>940</v>
       </c>
@@ -13507,7 +13647,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>940</v>
       </c>
@@ -13530,7 +13670,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
         <v>941</v>
       </c>
@@ -13553,7 +13693,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>942</v>
       </c>
@@ -13576,7 +13716,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
         <v>943</v>
       </c>
@@ -13599,7 +13739,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
         <v>944</v>
       </c>
@@ -13622,7 +13762,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
         <v>945</v>
       </c>
@@ -13678,8 +13818,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13824,7 +13964,7 @@
         <v>386</v>
       </c>
       <c r="D10" t="s">
-        <v>670</v>
+        <v>1176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>